<commit_message>
text display size is byte ,page2,3,4,12,14 text size changed
</commit_message>
<xml_diff>
--- a/MolecularDwinVariable.xlsx
+++ b/MolecularDwinVariable.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE0833E7-C2B7-4019-80F7-14FDE9E64044}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="97">
   <si>
     <t>文本变量</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -130,10 +129,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PAGE24</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PAGE25</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -163,11 +158,6 @@
   </si>
   <si>
     <t>PAGE31</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1000~1080   (256字节)                             
-1080~1100（256字节）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -182,34 +172,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>100 (4b) 610(4b)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100(4b) 610(4b)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">100(4b) 102(4b) </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>620(4b) 622(4b) 624(4b) 626(4b) 628(4b) 62A(4b) 62C(4b) 62E(4b) 630(4b) 632(4b) 634(4b) 636(4b) 638(4b) 63A(4b) 63C(4b) 63E(4b) 640(4b) 642(4b) 644(4b) 646(4b) 648(4b) 64A(4b) 64C(4b) 64E(4b) 650(4b) 652(4b) 654(4b) 656(4b)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>610(4b)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>700(4b)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>710(4b) 712(4b) 714(4b) 716(4b) 718(4b) 71A(4b)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>430(2b) 431(2b) 432(2b) 433(2b) 434(2b) 435(2b) 436(2b) 437(2b) 438(2b) 400(2b) 401(2b) 402(2b) 403(2b) 404(2b) 405(2b)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -219,26 +185,6 @@
   </si>
   <si>
     <t>100(4b) 102(4b)  110(4b) 112(4b) 610(4b)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>没有用到</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100 102 610   110 112 没有用到</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>440~46F 430~438 没有用到</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100(4b) 102(4b) 610(4b)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100(4b) 610(4b)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -271,66 +217,86 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1300~13C0  (384b)   13C0～1400 (128b)      2000～2010 (32b)     2010～2020(32b)     2020～2030 (32b)     2030～2040(32b)
-2040～2050 (32b)     2050-2060(32b)     1900 - 1950 (32b)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1400~1500 (512b)  13C0～1400(128b)   2000～2010(32b)    2010～2020 (32b)      2020～2030(32b)    2030～2040(32b)
-2040～2050(32b)   2050-2060(32b)       1900 - 1950 (32b)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1500~1600 (512b)  13C0～1400(128b)   2000～2010(32b)    2010～2020 (32b)      2020～2030(32b)    2030～2040(32b)
-2040～2050(32b)    2050-2060(32b)       1900 - 1950 (32b)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1600~1700 (512b) 13C0～1400(128b)    2000～2010(32b)    2010～2020 (32b)      2020～2030(32b)    2030～2040(32b)
-2040～2050(32b)    2050-2060(32b)       1900 - 1950 (32b)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1800~1900 (512b)  13C0～1400(128b)    2000～2010(32b)    2010～2020 (32b)      2020～2030(32b)    2030～2040(32b)
-2040～2050(32b)    2050-2060(32b)          1900 - 1950 (32b)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1800~1900 (512b)  13C0～1400(128b)    2000～2010(32b)    2010～2020 (32b)      2020～2030(32b)    2030～2040(32b)
-2040～2050(32b)    2050-2060(32b)        1900 - 1950 (32b)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1800~1900 (512b)  13C0～1400(128b)    2000～2010(32b)    2010～2020 (32b)      2020～2030(32b)    2030～2040(32b)
-2040～2050(32b)    2050-2060(32b)       1900 - 1950 (32b)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PAGE34</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>0x2280-22C0(128Byte)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x22C0-2300(128Byte)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>406(2b) 407(2b)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>弹出菜单</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAGE36</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAGE35</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAGE 37</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>418-428</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>120(4b)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1000~1080 (256字节)                            1080~1100（256字节）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>1100~1040（128b）
 1140~1080（128b）
 1080~11C0（128b）
-11C0~1200（128b）1200~1300（512b）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1800~1900 (512b)  13C0～1400(128b)    2000～2010(32b)    2010～2020 (32b)      2020～2030(32b)    2030～2040(32b)
-2040～2050(32b)    2050 -2060(32b)         1900 - 1950 (32b)   2400 - 2410</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x22C0-2300(128Byte)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>406(2b) 407(2b)</t>
+11C0~1200（128b）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1300~13C0  (384b)   13C0~1400 (128b)      2000~2060 (32b*6)   1900~1960 (32b*6)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1400~1500 (512b)  13C0～1400(128b)   2000~2060(32*6b)  1900~1950 (32b)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1500~1600 (512b)  13C0～1400(128b)  2000~2060(32*6b) 1900 - 1960 (32*6b)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1600~1700 (512b)  13C0～1400(128b)  2000~2060(32*6b)  1900~1960 (32*6b)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1700~1800 (512b)  13C0～1400(128b)  2000~2060(32*6b)  1900~1960 (32*6b) 1200~1240(128b)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1240~1280(128b)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1800~1900 (512b)  13C0～1400(128b)    2000～2060(32b*6) 1900~1960 (32b*6)   2400 - 2410(32b)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13C0～1400(128b)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -338,75 +304,123 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>弹出菜单</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PAGE36</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PAGE35</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x2500_0x2700</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>800(4byte)802 804 806 808 80A-81C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>81C(4b)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2420～2428</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100(4b) 610(4b)(81C)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PAGE 37</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0x2440~0x2480(128)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>600 (4b) 602(4b) 604(4b) 606(4b) 608(4b) 60A (4b) 60C(4b) 60E(4b)  610(4b)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>418-428</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>680(4b) 682(4b) 684(4b) 686(4b) 688(4b) 68A(4b) 68C(4b)68E(4b)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>120(4b)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>660(4b) 662(4b) 664(4b) 666(4b) 668(4b) 66A(4b) 66C(4b) 66E(4b) 670(4b) 672(4b)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>480-487</t>
+    <t>0x2500~0x2900(2048b)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAGE46</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAGE47</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAGE48</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x2900~0x2D00(2048b)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x2D00~0x3100(2048b)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x3100~0x3500(2048b)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100 (4b) 81C(4b)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>620~656(4b*28)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>620~656(4b*28)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>660~672(4b*10)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>660~672(4b*10)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>700(4b)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>710~71A(4b*6)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>710~71A(4b*6)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100 (4b) 81C(4b) 610(4b)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>800~81C(14*4b)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>600~60E(4b*7)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>600~60E(4b*7)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">610(4b) 680~68E(4b*8) </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">680~68E(4b*8) </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100 (4b) 81C(4b)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100 (4b) 81C(4b) 610(4b)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100(4b) 102(4b)  110(4b) 112(4b) 610(4b)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>430(2b) 431(2b) 432(2b) 433(2b) 434(2b) 435(2b) 436(2b) 437(2b) 438(2b) 400(2b) 401(2b) 402(2b) 403(2b) 404(2b) 405(2b)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>480-485</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RTC</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -442,7 +456,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -450,6 +464,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -729,21 +744,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R164"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34:M37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="5" max="5" width="15.125" customWidth="1"/>
     <col min="8" max="9" width="9" customWidth="1"/>
     <col min="17" max="17" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -769,15 +784,18 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+      <c r="S1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -795,7 +813,7 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -814,7 +832,7 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -833,7 +851,7 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -852,12 +870,12 @@
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -876,7 +894,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -896,7 +914,7 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -916,7 +934,7 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -936,12 +954,12 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" ht="22.5" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -960,7 +978,7 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -980,7 +998,7 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1000,7 +1018,7 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1020,24 +1038,24 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>39</v>
+        <v>85</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -1048,7 +1066,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1068,7 +1086,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1088,7 +1106,7 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="1:18" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" ht="41.25" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1108,17 +1126,17 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>81</v>
-      </c>
+      <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -1127,14 +1145,14 @@
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1154,7 +1172,7 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1174,7 +1192,7 @@
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1194,7 +1212,7 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -1216,7 +1234,7 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1236,7 +1254,7 @@
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1256,7 +1274,7 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1276,7 +1294,7 @@
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18">
       <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
@@ -1298,7 +1316,7 @@
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1318,7 +1336,7 @@
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1338,7 +1356,7 @@
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1358,24 +1376,24 @@
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18">
       <c r="A30" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
@@ -1386,7 +1404,7 @@
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1406,7 +1424,7 @@
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1426,7 +1444,7 @@
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
     </row>
-    <row r="33" spans="1:18" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:19" ht="39" customHeight="1">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1446,24 +1464,24 @@
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:19">
       <c r="A34" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
@@ -1474,7 +1492,7 @@
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:19">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1494,7 +1512,7 @@
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:19">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1514,7 +1532,7 @@
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
     </row>
-    <row r="37" spans="1:18" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:19" ht="67.5" customHeight="1">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1534,24 +1552,24 @@
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:19">
       <c r="A38" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
@@ -1562,7 +1580,7 @@
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:19">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1582,7 +1600,7 @@
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:19">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1602,7 +1620,7 @@
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
     </row>
-    <row r="41" spans="1:18" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:19" ht="41.25" customHeight="1">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1622,7 +1640,7 @@
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:19">
       <c r="A42" s="1" t="s">
         <v>14</v>
       </c>
@@ -1635,7 +1653,7 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
@@ -1646,7 +1664,7 @@
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:19">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1666,7 +1684,7 @@
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:19">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1686,7 +1704,7 @@
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:19">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1706,7 +1724,7 @@
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:19">
       <c r="A46" s="1" t="s">
         <v>15</v>
       </c>
@@ -1717,13 +1735,13 @@
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
@@ -1735,8 +1753,11 @@
       <c r="R46" s="1">
         <v>300</v>
       </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S46" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1755,8 +1776,9 @@
       <c r="P47" s="1"/>
       <c r="Q47" s="1"/>
       <c r="R47" s="1"/>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S47" s="3"/>
+    </row>
+    <row r="48" spans="1:19">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1775,8 +1797,9 @@
       <c r="P48" s="1"/>
       <c r="Q48" s="1"/>
       <c r="R48" s="1"/>
-    </row>
-    <row r="49" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S48" s="3"/>
+    </row>
+    <row r="49" spans="1:19" ht="32.25" customHeight="1">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1795,8 +1818,9 @@
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
       <c r="R49" s="1"/>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S49" s="3"/>
+    </row>
+    <row r="50" spans="1:19">
       <c r="A50" s="1" t="s">
         <v>16</v>
       </c>
@@ -1809,7 +1833,7 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
       <c r="J50" s="1" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
@@ -1820,7 +1844,7 @@
       <c r="Q50" s="1"/>
       <c r="R50" s="1"/>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:19">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1840,7 +1864,7 @@
       <c r="Q51" s="1"/>
       <c r="R51" s="1"/>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:19">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1860,7 +1884,7 @@
       <c r="Q52" s="1"/>
       <c r="R52" s="1"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:19">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1880,11 +1904,13 @@
       <c r="Q53" s="1"/>
       <c r="R53" s="1"/>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:19">
       <c r="A54" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B54" s="1"/>
+      <c r="B54" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
@@ -1902,7 +1928,7 @@
       <c r="Q54" s="1"/>
       <c r="R54" s="1"/>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:19">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1922,7 +1948,7 @@
       <c r="Q55" s="1"/>
       <c r="R55" s="1"/>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:19">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1942,7 +1968,7 @@
       <c r="Q56" s="1"/>
       <c r="R56" s="1"/>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:19">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1962,7 +1988,7 @@
       <c r="Q57" s="1"/>
       <c r="R57" s="1"/>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:19">
       <c r="A58" s="1" t="s">
         <v>18</v>
       </c>
@@ -1970,7 +1996,9 @@
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
+      <c r="F58" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
@@ -1979,14 +2007,14 @@
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
       <c r="N58" s="1" t="s">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="O58" s="1"/>
       <c r="P58" s="1"/>
       <c r="Q58" s="1"/>
       <c r="R58" s="1"/>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:19">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2006,7 +2034,7 @@
       <c r="Q59" s="1"/>
       <c r="R59" s="1"/>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:19">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2026,7 +2054,7 @@
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:19" ht="39.75" customHeight="1">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2046,7 +2074,7 @@
       <c r="Q61" s="1"/>
       <c r="R61" s="1"/>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:19">
       <c r="A62" s="1" t="s">
         <v>19</v>
       </c>
@@ -2054,7 +2082,9 @@
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
+      <c r="F62" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
@@ -2063,14 +2093,14 @@
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
       <c r="N62" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="O62" s="1"/>
       <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
       <c r="R62" s="1"/>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:19">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2090,7 +2120,7 @@
       <c r="Q63" s="1"/>
       <c r="R63" s="1"/>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:19">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2110,7 +2140,7 @@
       <c r="Q64" s="1"/>
       <c r="R64" s="1"/>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:18">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -2130,7 +2160,7 @@
       <c r="Q65" s="1"/>
       <c r="R65" s="1"/>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:18">
       <c r="A66" s="1" t="s">
         <v>20</v>
       </c>
@@ -2139,7 +2169,7 @@
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
@@ -2149,14 +2179,14 @@
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
       <c r="N66" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="O66" s="1"/>
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
       <c r="R66" s="1"/>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:18">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2176,7 +2206,7 @@
       <c r="Q67" s="1"/>
       <c r="R67" s="1"/>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:18">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2196,7 +2226,7 @@
       <c r="Q68" s="1"/>
       <c r="R68" s="1"/>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:18">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2216,7 +2246,7 @@
       <c r="Q69" s="1"/>
       <c r="R69" s="1"/>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:18">
       <c r="A70" s="1" t="s">
         <v>21</v>
       </c>
@@ -2225,7 +2255,7 @@
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1" t="s">
-        <v>88</v>
+        <v>57</v>
       </c>
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
@@ -2240,7 +2270,7 @@
       <c r="Q70" s="1"/>
       <c r="R70" s="1"/>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:18">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2260,7 +2290,7 @@
       <c r="Q71" s="1"/>
       <c r="R71" s="1"/>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:18">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2280,7 +2310,7 @@
       <c r="Q72" s="1"/>
       <c r="R72" s="1"/>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:18">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2300,7 +2330,7 @@
       <c r="Q73" s="1"/>
       <c r="R73" s="1"/>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:18">
       <c r="A74" s="1" t="s">
         <v>22</v>
       </c>
@@ -2308,7 +2338,9 @@
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
+      <c r="F74" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
@@ -2317,14 +2349,14 @@
       <c r="L74" s="1"/>
       <c r="M74" s="1"/>
       <c r="N74" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="O74" s="1"/>
       <c r="P74" s="1"/>
       <c r="Q74" s="1"/>
       <c r="R74" s="1"/>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:18">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -2344,7 +2376,7 @@
       <c r="Q75" s="1"/>
       <c r="R75" s="1"/>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:18">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -2364,7 +2396,7 @@
       <c r="Q76" s="1"/>
       <c r="R76" s="1"/>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:18">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -2384,7 +2416,7 @@
       <c r="Q77" s="1"/>
       <c r="R77" s="1"/>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:18">
       <c r="A78" s="1" t="s">
         <v>23</v>
       </c>
@@ -2392,7 +2424,9 @@
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
-      <c r="F78" s="1"/>
+      <c r="F78" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
@@ -2401,14 +2435,14 @@
       <c r="L78" s="1"/>
       <c r="M78" s="1"/>
       <c r="N78" s="1" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="O78" s="1"/>
       <c r="P78" s="1"/>
       <c r="Q78" s="1"/>
       <c r="R78" s="1"/>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:18">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2428,7 +2462,7 @@
       <c r="Q79" s="1"/>
       <c r="R79" s="1"/>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:18">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2448,7 +2482,7 @@
       <c r="Q80" s="1"/>
       <c r="R80" s="1"/>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:18">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2468,35 +2502,37 @@
       <c r="Q81" s="1"/>
       <c r="R81" s="1"/>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:18">
       <c r="A82" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
       <c r="F82" s="1" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
       <c r="J82" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="K82" s="1"/>
       <c r="L82" s="1"/>
       <c r="M82" s="1"/>
-      <c r="N82" s="1"/>
+      <c r="N82" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="O82" s="1"/>
       <c r="P82" s="1"/>
       <c r="Q82" s="1"/>
       <c r="R82" s="1"/>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:18">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2516,7 +2552,7 @@
       <c r="Q83" s="1"/>
       <c r="R83" s="1"/>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:18">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2536,7 +2572,7 @@
       <c r="Q84" s="1"/>
       <c r="R84" s="1"/>
     </row>
-    <row r="85" spans="1:18" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:18" ht="54.75" customHeight="1">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2556,35 +2592,37 @@
       <c r="Q85" s="1"/>
       <c r="R85" s="1"/>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:18">
       <c r="A86" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
       <c r="F86" s="1" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
       <c r="J86" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="K86" s="1"/>
       <c r="L86" s="1"/>
       <c r="M86" s="1"/>
-      <c r="N86" s="1"/>
+      <c r="N86" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="O86" s="1"/>
       <c r="P86" s="1"/>
       <c r="Q86" s="1"/>
       <c r="R86" s="1"/>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:18">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -2604,7 +2642,7 @@
       <c r="Q87" s="1"/>
       <c r="R87" s="1"/>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:18">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -2624,7 +2662,7 @@
       <c r="Q88" s="1"/>
       <c r="R88" s="1"/>
     </row>
-    <row r="89" spans="1:18" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:18" ht="37.5" customHeight="1">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -2644,33 +2682,37 @@
       <c r="Q89" s="1"/>
       <c r="R89" s="1"/>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:18" ht="13.5" customHeight="1">
       <c r="A90" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B90" s="1"/>
+      <c r="B90" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
       <c r="F90" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G90" s="1"/>
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
       <c r="J90" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="K90" s="1"/>
       <c r="L90" s="1"/>
       <c r="M90" s="1"/>
-      <c r="N90" s="1"/>
+      <c r="N90" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="O90" s="1"/>
       <c r="P90" s="1"/>
       <c r="Q90" s="1"/>
       <c r="R90" s="1"/>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:18">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -2690,7 +2732,7 @@
       <c r="Q91" s="1"/>
       <c r="R91" s="1"/>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:18">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -2710,7 +2752,7 @@
       <c r="Q92" s="1"/>
       <c r="R92" s="1"/>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:18">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -2730,25 +2772,17 @@
       <c r="Q93" s="1"/>
       <c r="R93" s="1"/>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A94" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>49</v>
-      </c>
+    <row r="94" spans="1:18">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
-      <c r="F94" s="1" t="s">
-        <v>50</v>
-      </c>
+      <c r="F94" s="1"/>
       <c r="G94" s="1"/>
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
-      <c r="J94" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="J94" s="1"/>
       <c r="K94" s="1"/>
       <c r="L94" s="1"/>
       <c r="M94" s="1"/>
@@ -2758,7 +2792,7 @@
       <c r="Q94" s="1"/>
       <c r="R94" s="1"/>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:18">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -2778,7 +2812,7 @@
       <c r="Q95" s="1"/>
       <c r="R95" s="1"/>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:18">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -2798,7 +2832,7 @@
       <c r="Q96" s="1"/>
       <c r="R96" s="1"/>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:18">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -2818,9 +2852,9 @@
       <c r="Q97" s="1"/>
       <c r="R97" s="1"/>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:18">
       <c r="A98" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>66</v>
@@ -2829,24 +2863,26 @@
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
       <c r="F98" s="1" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="G98" s="1"/>
       <c r="H98" s="1"/>
       <c r="I98" s="1"/>
       <c r="J98" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="K98" s="1"/>
       <c r="L98" s="1"/>
       <c r="M98" s="1"/>
-      <c r="N98" s="1"/>
+      <c r="N98" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="O98" s="1"/>
       <c r="P98" s="1"/>
       <c r="Q98" s="1"/>
       <c r="R98" s="1"/>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:18">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -2866,7 +2902,7 @@
       <c r="Q99" s="1"/>
       <c r="R99" s="1"/>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:18">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -2886,7 +2922,7 @@
       <c r="Q100" s="1"/>
       <c r="R100" s="1"/>
     </row>
-    <row r="101" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:18" ht="50.25" customHeight="1">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -2906,33 +2942,37 @@
       <c r="Q101" s="1"/>
       <c r="R101" s="1"/>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:18">
       <c r="A102" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
       <c r="F102" s="1" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="G102" s="1"/>
       <c r="H102" s="1"/>
       <c r="I102" s="1"/>
-      <c r="J102" s="1"/>
+      <c r="J102" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="K102" s="1"/>
       <c r="L102" s="1"/>
       <c r="M102" s="1"/>
-      <c r="N102" s="1"/>
+      <c r="N102" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="O102" s="1"/>
       <c r="P102" s="1"/>
       <c r="Q102" s="1"/>
       <c r="R102" s="1"/>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:18">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -2952,7 +2992,7 @@
       <c r="Q103" s="1"/>
       <c r="R103" s="1"/>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:18">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -2972,7 +3012,7 @@
       <c r="Q104" s="1"/>
       <c r="R104" s="1"/>
     </row>
-    <row r="105" spans="1:18" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:18" ht="39" customHeight="1">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -2992,9 +3032,9 @@
       <c r="Q105" s="1"/>
       <c r="R105" s="1"/>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:18">
       <c r="A106" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -3014,7 +3054,7 @@
       <c r="Q106" s="1"/>
       <c r="R106" s="1"/>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:18">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -3034,7 +3074,7 @@
       <c r="Q107" s="1"/>
       <c r="R107" s="1"/>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:18">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -3054,7 +3094,7 @@
       <c r="Q108" s="1"/>
       <c r="R108" s="1"/>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:18">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -3074,12 +3114,12 @@
       <c r="Q109" s="1"/>
       <c r="R109" s="1"/>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:18">
       <c r="A110" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
@@ -3098,7 +3138,7 @@
       <c r="Q110" s="1"/>
       <c r="R110" s="1"/>
     </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:18">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -3118,7 +3158,7 @@
       <c r="Q111" s="1"/>
       <c r="R111" s="1"/>
     </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:18">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -3138,7 +3178,7 @@
       <c r="Q112" s="1"/>
       <c r="R112" s="1"/>
     </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:18">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -3158,12 +3198,12 @@
       <c r="Q113" s="1"/>
       <c r="R113" s="1"/>
     </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:18">
       <c r="A114" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
@@ -3182,7 +3222,7 @@
       <c r="Q114" s="1"/>
       <c r="R114" s="1"/>
     </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:18">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -3202,7 +3242,7 @@
       <c r="Q115" s="1"/>
       <c r="R115" s="1"/>
     </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:18">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -3222,7 +3262,7 @@
       <c r="Q116" s="1"/>
       <c r="R116" s="1"/>
     </row>
-    <row r="117" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:18">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -3242,12 +3282,12 @@
       <c r="Q117" s="1"/>
       <c r="R117" s="1"/>
     </row>
-    <row r="118" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:18">
       <c r="A118" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
@@ -3266,7 +3306,7 @@
       <c r="Q118" s="1"/>
       <c r="R118" s="1"/>
     </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:18">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -3286,7 +3326,7 @@
       <c r="Q119" s="1"/>
       <c r="R119" s="1"/>
     </row>
-    <row r="120" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:18">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -3306,7 +3346,7 @@
       <c r="Q120" s="1"/>
       <c r="R120" s="1"/>
     </row>
-    <row r="121" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:18">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -3326,12 +3366,12 @@
       <c r="Q121" s="1"/>
       <c r="R121" s="1"/>
     </row>
-    <row r="122" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:18">
       <c r="A122" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
@@ -3350,7 +3390,7 @@
       <c r="Q122" s="1"/>
       <c r="R122" s="1"/>
     </row>
-    <row r="123" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:18">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -3370,7 +3410,7 @@
       <c r="Q123" s="1"/>
       <c r="R123" s="1"/>
     </row>
-    <row r="124" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:18">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -3390,7 +3430,7 @@
       <c r="Q124" s="1"/>
       <c r="R124" s="1"/>
     </row>
-    <row r="125" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:18">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -3410,12 +3450,12 @@
       <c r="Q125" s="1"/>
       <c r="R125" s="1"/>
     </row>
-    <row r="126" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:18">
       <c r="A126" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
@@ -3434,7 +3474,7 @@
       <c r="Q126" s="1"/>
       <c r="R126" s="1"/>
     </row>
-    <row r="127" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:18">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -3454,7 +3494,7 @@
       <c r="Q127" s="1"/>
       <c r="R127" s="1"/>
     </row>
-    <row r="128" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:18">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -3474,7 +3514,7 @@
       <c r="Q128" s="1"/>
       <c r="R128" s="1"/>
     </row>
-    <row r="129" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:18">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -3494,12 +3534,12 @@
       <c r="Q129" s="1"/>
       <c r="R129" s="1"/>
     </row>
-    <row r="130" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:18">
       <c r="A130" s="2" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="C130" s="1"/>
       <c r="D130" s="1"/>
@@ -3518,7 +3558,7 @@
       <c r="Q130" s="1"/>
       <c r="R130" s="1"/>
     </row>
-    <row r="131" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:18">
       <c r="A131" s="2"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -3538,7 +3578,7 @@
       <c r="Q131" s="1"/>
       <c r="R131" s="1"/>
     </row>
-    <row r="132" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:18">
       <c r="A132" s="2"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -3558,7 +3598,7 @@
       <c r="Q132" s="1"/>
       <c r="R132" s="1"/>
     </row>
-    <row r="133" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:18">
       <c r="A133" s="2"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -3578,12 +3618,12 @@
       <c r="Q133" s="1"/>
       <c r="R133" s="1"/>
     </row>
-    <row r="134" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:18">
       <c r="A134" s="2" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="C134" s="1"/>
       <c r="D134" s="1"/>
@@ -3602,7 +3642,7 @@
       <c r="Q134" s="1"/>
       <c r="R134" s="1"/>
     </row>
-    <row r="135" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:18">
       <c r="A135" s="2"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -3622,7 +3662,7 @@
       <c r="Q135" s="1"/>
       <c r="R135" s="1"/>
     </row>
-    <row r="136" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:18">
       <c r="A136" s="2"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -3642,7 +3682,7 @@
       <c r="Q136" s="1"/>
       <c r="R136" s="1"/>
     </row>
-    <row r="137" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:18">
       <c r="A137" s="2"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -3662,12 +3702,12 @@
       <c r="Q137" s="1"/>
       <c r="R137" s="1"/>
     </row>
-    <row r="138" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:18">
       <c r="A138" s="2" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="C138" s="1"/>
       <c r="D138" s="1"/>
@@ -3686,7 +3726,7 @@
       <c r="Q138" s="1"/>
       <c r="R138" s="1"/>
     </row>
-    <row r="139" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:18">
       <c r="A139" s="2"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -3706,7 +3746,7 @@
       <c r="Q139" s="1"/>
       <c r="R139" s="1"/>
     </row>
-    <row r="140" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:18">
       <c r="A140" s="2"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -3726,7 +3766,7 @@
       <c r="Q140" s="1"/>
       <c r="R140" s="1"/>
     </row>
-    <row r="141" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:18">
       <c r="A141" s="2"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -3746,7 +3786,7 @@
       <c r="Q141" s="1"/>
       <c r="R141" s="1"/>
     </row>
-    <row r="142" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:18">
       <c r="A142" s="2"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -3766,35 +3806,35 @@
       <c r="Q142" s="1"/>
       <c r="R142" s="1"/>
     </row>
-    <row r="143" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:18">
       <c r="A143" s="2" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
       <c r="D143" s="1"/>
       <c r="E143" s="1"/>
       <c r="F143" s="1" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="G143" s="1"/>
       <c r="H143" s="1"/>
       <c r="I143" s="1"/>
       <c r="J143" s="1" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="K143" s="1"/>
       <c r="L143" s="1"/>
       <c r="M143" s="1"/>
       <c r="N143" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="O143" s="1"/>
       <c r="P143" s="1"/>
       <c r="Q143" s="1"/>
       <c r="R143" s="1"/>
     </row>
-    <row r="144" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:18">
       <c r="A144" s="2"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -3814,7 +3854,7 @@
       <c r="Q144" s="1"/>
       <c r="R144" s="1"/>
     </row>
-    <row r="145" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:18">
       <c r="A145" s="2"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -3834,7 +3874,7 @@
       <c r="Q145" s="1"/>
       <c r="R145" s="1"/>
     </row>
-    <row r="146" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:18">
       <c r="A146" s="2"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -3854,12 +3894,12 @@
       <c r="Q146" s="1"/>
       <c r="R146" s="1"/>
     </row>
-    <row r="147" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:18">
       <c r="A147" s="2" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C147" s="1"/>
       <c r="D147" s="1"/>
@@ -3878,7 +3918,7 @@
       <c r="Q147" s="1"/>
       <c r="R147" s="1"/>
     </row>
-    <row r="148" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:18">
       <c r="A148" s="2"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -3898,7 +3938,7 @@
       <c r="Q148" s="1"/>
       <c r="R148" s="1"/>
     </row>
-    <row r="149" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:18">
       <c r="A149" s="2"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -3918,7 +3958,7 @@
       <c r="Q149" s="1"/>
       <c r="R149" s="1"/>
     </row>
-    <row r="150" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:18">
       <c r="A150" s="2"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -3936,14 +3976,13 @@
       <c r="O150" s="1"/>
       <c r="P150" s="1"/>
       <c r="Q150" s="1"/>
-      <c r="R150" s="1"/>
-    </row>
-    <row r="151" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="151" spans="1:18">
       <c r="A151" s="2" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C151" s="1"/>
       <c r="D151" s="1"/>
@@ -3960,9 +3999,8 @@
       <c r="O151" s="1"/>
       <c r="P151" s="1"/>
       <c r="Q151" s="1"/>
-      <c r="R151" s="1"/>
-    </row>
-    <row r="152" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="152" spans="1:18">
       <c r="A152" s="2"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -3980,9 +4018,8 @@
       <c r="O152" s="1"/>
       <c r="P152" s="1"/>
       <c r="Q152" s="1"/>
-      <c r="R152" s="1"/>
-    </row>
-    <row r="153" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="153" spans="1:18">
       <c r="A153" s="2"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -4000,9 +4037,8 @@
       <c r="O153" s="1"/>
       <c r="P153" s="1"/>
       <c r="Q153" s="1"/>
-      <c r="R153" s="1"/>
-    </row>
-    <row r="154" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="154" spans="1:18">
       <c r="A154" s="2"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -4021,9 +4057,13 @@
       <c r="P154" s="1"/>
       <c r="Q154" s="1"/>
     </row>
-    <row r="155" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A155" s="2"/>
-      <c r="B155" s="1"/>
+    <row r="155" spans="1:18">
+      <c r="A155" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="C155" s="1"/>
       <c r="D155" s="1"/>
       <c r="E155" s="1"/>
@@ -4040,7 +4080,7 @@
       <c r="P155" s="1"/>
       <c r="Q155" s="1"/>
     </row>
-    <row r="156" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:18">
       <c r="A156" s="2"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -4059,7 +4099,7 @@
       <c r="P156" s="1"/>
       <c r="Q156" s="1"/>
     </row>
-    <row r="157" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:18">
       <c r="A157" s="2"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -4078,7 +4118,7 @@
       <c r="P157" s="1"/>
       <c r="Q157" s="1"/>
     </row>
-    <row r="158" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:18">
       <c r="A158" s="2"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -4097,9 +4137,13 @@
       <c r="P158" s="1"/>
       <c r="Q158" s="1"/>
     </row>
-    <row r="159" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A159" s="2"/>
-      <c r="B159" s="1"/>
+    <row r="159" spans="1:18">
+      <c r="A159" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="C159" s="1"/>
       <c r="D159" s="1"/>
       <c r="E159" s="1"/>
@@ -4116,7 +4160,7 @@
       <c r="P159" s="1"/>
       <c r="Q159" s="1"/>
     </row>
-    <row r="160" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:18">
       <c r="A160" s="2"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -4135,103 +4179,55 @@
       <c r="P160" s="1"/>
       <c r="Q160" s="1"/>
     </row>
-    <row r="161" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A161" s="2"/>
-      <c r="B161" s="1"/>
-      <c r="C161" s="1"/>
-      <c r="D161" s="1"/>
-      <c r="E161" s="1"/>
-      <c r="F161" s="1"/>
-      <c r="G161" s="1"/>
-      <c r="H161" s="1"/>
-      <c r="I161" s="1"/>
-      <c r="J161" s="1"/>
-      <c r="K161" s="1"/>
-      <c r="L161" s="1"/>
-      <c r="M161" s="1"/>
-      <c r="N161" s="1"/>
-      <c r="O161" s="1"/>
-      <c r="P161" s="1"/>
-      <c r="Q161" s="1"/>
-    </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A162" s="2"/>
-      <c r="B162" s="1"/>
-      <c r="C162" s="1"/>
-      <c r="D162" s="1"/>
-      <c r="E162" s="1"/>
-      <c r="F162" s="1"/>
-      <c r="G162" s="1"/>
-      <c r="H162" s="1"/>
-      <c r="I162" s="1"/>
-      <c r="J162" s="1"/>
-      <c r="K162" s="1"/>
-      <c r="L162" s="1"/>
-      <c r="M162" s="1"/>
-      <c r="N162" s="1"/>
-      <c r="O162" s="1"/>
-      <c r="P162" s="1"/>
-      <c r="Q162" s="1"/>
-    </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A163" s="2"/>
-      <c r="B163" s="1"/>
-      <c r="C163" s="1"/>
-      <c r="D163" s="1"/>
-      <c r="E163" s="1"/>
-      <c r="F163" s="1"/>
-      <c r="G163" s="1"/>
-      <c r="H163" s="1"/>
-      <c r="I163" s="1"/>
-      <c r="J163" s="1"/>
-      <c r="K163" s="1"/>
-      <c r="L163" s="1"/>
-      <c r="M163" s="1"/>
-      <c r="N163" s="1"/>
-      <c r="O163" s="1"/>
-      <c r="P163" s="1"/>
-      <c r="Q163" s="1"/>
-    </row>
-    <row r="164" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A164" s="2"/>
-      <c r="B164" s="1"/>
-      <c r="C164" s="1"/>
-      <c r="D164" s="1"/>
-      <c r="E164" s="1"/>
-      <c r="F164" s="1"/>
-      <c r="G164" s="1"/>
-      <c r="H164" s="1"/>
-      <c r="I164" s="1"/>
-      <c r="J164" s="1"/>
-      <c r="K164" s="1"/>
-      <c r="L164" s="1"/>
-      <c r="M164" s="1"/>
-      <c r="N164" s="1"/>
-      <c r="O164" s="1"/>
-      <c r="P164" s="1"/>
-      <c r="Q164" s="1"/>
+    <row r="161" spans="1:17">
+      <c r="A161" t="s">
+        <v>73</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C161" s="2"/>
+      <c r="D161" s="2"/>
+      <c r="E161" s="2"/>
+      <c r="F161" s="2"/>
+      <c r="G161" s="2"/>
+      <c r="H161" s="2"/>
+      <c r="I161" s="2"/>
+      <c r="J161" s="2"/>
+      <c r="K161" s="2"/>
+      <c r="L161" s="2"/>
+      <c r="M161" s="2"/>
+      <c r="N161" s="2"/>
+      <c r="O161" s="2"/>
+      <c r="P161" s="2"/>
+      <c r="Q161" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="246">
-    <mergeCell ref="A159:A162"/>
-    <mergeCell ref="B159:E162"/>
-    <mergeCell ref="F159:I162"/>
-    <mergeCell ref="J159:M162"/>
-    <mergeCell ref="N159:Q162"/>
-    <mergeCell ref="A163:A164"/>
-    <mergeCell ref="B163:E164"/>
-    <mergeCell ref="F163:I164"/>
-    <mergeCell ref="J163:M164"/>
-    <mergeCell ref="N163:Q164"/>
-    <mergeCell ref="A151:A154"/>
-    <mergeCell ref="B151:E154"/>
-    <mergeCell ref="J151:M154"/>
-    <mergeCell ref="N151:Q154"/>
+  <mergeCells count="245">
+    <mergeCell ref="B161:E161"/>
+    <mergeCell ref="F161:I161"/>
+    <mergeCell ref="J161:M161"/>
+    <mergeCell ref="N161:Q161"/>
+    <mergeCell ref="S46:S49"/>
     <mergeCell ref="A155:A158"/>
     <mergeCell ref="B155:E158"/>
     <mergeCell ref="F155:I158"/>
     <mergeCell ref="J155:M158"/>
     <mergeCell ref="N155:Q158"/>
+    <mergeCell ref="A159:A160"/>
+    <mergeCell ref="B159:E160"/>
+    <mergeCell ref="F159:I160"/>
+    <mergeCell ref="J159:M160"/>
+    <mergeCell ref="N159:Q160"/>
+    <mergeCell ref="A147:A150"/>
+    <mergeCell ref="B147:E150"/>
+    <mergeCell ref="J147:M150"/>
+    <mergeCell ref="N147:Q150"/>
+    <mergeCell ref="A151:A154"/>
+    <mergeCell ref="B151:E154"/>
+    <mergeCell ref="F151:I154"/>
+    <mergeCell ref="J151:M154"/>
+    <mergeCell ref="N151:Q154"/>
     <mergeCell ref="A134:A137"/>
     <mergeCell ref="B134:E137"/>
     <mergeCell ref="A138:A142"/>
@@ -4239,15 +4235,10 @@
     <mergeCell ref="A143:A146"/>
     <mergeCell ref="B143:E146"/>
     <mergeCell ref="J143:M146"/>
-    <mergeCell ref="A147:A150"/>
-    <mergeCell ref="B147:E150"/>
-    <mergeCell ref="J147:M150"/>
     <mergeCell ref="J138:M142"/>
     <mergeCell ref="N143:Q146"/>
     <mergeCell ref="R143:R146"/>
-    <mergeCell ref="N147:Q150"/>
-    <mergeCell ref="R147:R150"/>
-    <mergeCell ref="R151:R153"/>
+    <mergeCell ref="R147:R149"/>
     <mergeCell ref="N130:Q133"/>
     <mergeCell ref="R130:R133"/>
     <mergeCell ref="N134:Q137"/>
@@ -4333,7 +4324,6 @@
     <mergeCell ref="F138:I142"/>
     <mergeCell ref="F143:I146"/>
     <mergeCell ref="F147:I150"/>
-    <mergeCell ref="F151:I154"/>
     <mergeCell ref="F122:I125"/>
     <mergeCell ref="F126:I129"/>
     <mergeCell ref="J122:M125"/>
@@ -4382,7 +4372,6 @@
     <mergeCell ref="F38:I41"/>
     <mergeCell ref="J34:M37"/>
     <mergeCell ref="J38:M41"/>
-    <mergeCell ref="F26:I29"/>
     <mergeCell ref="F30:I33"/>
     <mergeCell ref="J30:M33"/>
     <mergeCell ref="F18:I21"/>
@@ -4440,14 +4429,6 @@
     <mergeCell ref="B42:E45"/>
     <mergeCell ref="A46:A49"/>
     <mergeCell ref="B46:E49"/>
-    <mergeCell ref="B22:E25"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:E29"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:E33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:E37"/>
-    <mergeCell ref="A22:A25"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E5"/>
     <mergeCell ref="B6:E9"/>
@@ -4459,6 +4440,15 @@
     <mergeCell ref="B18:E21"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A9"/>
+    <mergeCell ref="F26:I29"/>
+    <mergeCell ref="B22:E25"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B26:E29"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:E33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:E37"/>
+    <mergeCell ref="A22:A25"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
change all text lenght div 2
</commit_message>
<xml_diff>
--- a/MolecularDwinVariable.xlsx
+++ b/MolecularDwinVariable.xlsx
@@ -747,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34:M37"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B102" sqref="B102:E105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4263,6 +4263,9 @@
     <mergeCell ref="R98:R101"/>
     <mergeCell ref="N102:Q105"/>
     <mergeCell ref="R102:R105"/>
+    <mergeCell ref="R30:R33"/>
+    <mergeCell ref="N34:Q37"/>
+    <mergeCell ref="R34:R37"/>
     <mergeCell ref="N82:Q85"/>
     <mergeCell ref="R82:R85"/>
     <mergeCell ref="N86:Q89"/>
@@ -4274,6 +4277,24 @@
     <mergeCell ref="R74:R77"/>
     <mergeCell ref="N78:Q81"/>
     <mergeCell ref="R78:R81"/>
+    <mergeCell ref="R6:R9"/>
+    <mergeCell ref="N10:Q13"/>
+    <mergeCell ref="R10:R13"/>
+    <mergeCell ref="N14:Q17"/>
+    <mergeCell ref="R14:R17"/>
+    <mergeCell ref="N18:Q21"/>
+    <mergeCell ref="R18:R21"/>
+    <mergeCell ref="R22:R25"/>
+    <mergeCell ref="N26:Q29"/>
+    <mergeCell ref="R26:R29"/>
+    <mergeCell ref="R38:R41"/>
+    <mergeCell ref="N42:Q45"/>
+    <mergeCell ref="R42:R45"/>
+    <mergeCell ref="N46:Q49"/>
+    <mergeCell ref="R46:R49"/>
+    <mergeCell ref="N50:Q53"/>
+    <mergeCell ref="R50:R53"/>
+    <mergeCell ref="N70:Q73"/>
     <mergeCell ref="R54:R57"/>
     <mergeCell ref="N58:Q61"/>
     <mergeCell ref="R58:R61"/>
@@ -4281,30 +4302,6 @@
     <mergeCell ref="R62:R65"/>
     <mergeCell ref="N66:Q69"/>
     <mergeCell ref="R66:R69"/>
-    <mergeCell ref="R6:R9"/>
-    <mergeCell ref="N10:Q13"/>
-    <mergeCell ref="R10:R13"/>
-    <mergeCell ref="N14:Q17"/>
-    <mergeCell ref="R14:R17"/>
-    <mergeCell ref="N18:Q21"/>
-    <mergeCell ref="R18:R21"/>
-    <mergeCell ref="J130:M133"/>
-    <mergeCell ref="J134:M137"/>
-    <mergeCell ref="R38:R41"/>
-    <mergeCell ref="N42:Q45"/>
-    <mergeCell ref="R42:R45"/>
-    <mergeCell ref="N46:Q49"/>
-    <mergeCell ref="R46:R49"/>
-    <mergeCell ref="N50:Q53"/>
-    <mergeCell ref="R50:R53"/>
-    <mergeCell ref="R22:R25"/>
-    <mergeCell ref="N26:Q29"/>
-    <mergeCell ref="R26:R29"/>
-    <mergeCell ref="N30:Q33"/>
-    <mergeCell ref="R30:R33"/>
-    <mergeCell ref="N34:Q37"/>
-    <mergeCell ref="R34:R37"/>
-    <mergeCell ref="N70:Q73"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="N2:Q5"/>
     <mergeCell ref="N6:Q9"/>
@@ -4319,6 +4316,7 @@
     <mergeCell ref="J18:M21"/>
     <mergeCell ref="J22:M25"/>
     <mergeCell ref="J26:M29"/>
+    <mergeCell ref="N30:Q33"/>
     <mergeCell ref="F130:I133"/>
     <mergeCell ref="F134:I137"/>
     <mergeCell ref="F138:I142"/>
@@ -4328,6 +4326,8 @@
     <mergeCell ref="F126:I129"/>
     <mergeCell ref="J122:M125"/>
     <mergeCell ref="J126:M129"/>
+    <mergeCell ref="J130:M133"/>
+    <mergeCell ref="J134:M137"/>
     <mergeCell ref="F114:I117"/>
     <mergeCell ref="F118:I121"/>
     <mergeCell ref="J114:M117"/>

</xml_diff>